<commit_message>
lock the excel title row, change the attached file attribute, clear db data
</commit_message>
<xml_diff>
--- a/Limitless/LimitLess/Files/excel_format.xlsx
+++ b/Limitless/LimitLess/Files/excel_format.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26207"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Erin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADSIXPS15\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="15456"/>
   </bookViews>
   <sheets>
     <sheet name="Upload File" sheetId="1" r:id="rId1"/>
@@ -17,11 +17,11 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,9 +189,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -510,119 +521,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="15" width="21.5" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" customWidth="1"/>
-    <col min="17" max="17" width="23" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" customWidth="1"/>
-    <col min="19" max="20" width="21.5" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" customWidth="1"/>
-    <col min="22" max="22" width="23" customWidth="1"/>
-    <col min="23" max="23" width="17.6640625" customWidth="1"/>
-    <col min="24" max="25" width="21.5" customWidth="1"/>
-    <col min="26" max="26" width="24.5" customWidth="1"/>
-    <col min="27" max="27" width="33.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="24.44140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="23" style="2" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" style="2" customWidth="1"/>
+    <col min="15" max="16" width="21.44140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="23" style="2" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" style="2" customWidth="1"/>
+    <col min="20" max="21" width="21.44140625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="23" style="2" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" style="2" customWidth="1"/>
+    <col min="25" max="26" width="21.44140625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="33.77734375" style="2" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="pbGed6EHLGlsMPhUJ8HqKfHEEtdyi/YzgWQ4kEYOT4aycPUh8h5CCOXW0oMuqBPLQLG8Jab/hSnALWW9u98M6A==" saltValue="RpQXYio+JgFRYuE6ETqSNw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -662,7 +675,7 @@
           <x14:formula1>
             <xm:f>'Drop down items'!$H$1:$H$2</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:O1048576 S2:T1048576 X2:Y1048576 J2:J1048576</xm:sqref>
+          <xm:sqref>O2:P1048576 T2:U1048576 Y2:Z1048576 J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -690,18 +703,18 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="36.1640625" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="36.109375" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -727,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -753,7 +766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -773,7 +786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>

</xml_diff>